<commit_message>
main table preparation 2
</commit_message>
<xml_diff>
--- a/_data/database_tables_upgrades.xlsx
+++ b/_data/database_tables_upgrades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00201d7a97493cc5/web_projects/norman-db/_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_w\norman-db\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{066A7533-50EC-4B34-8D2C-2D7371F53900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27D68D80-B431-4D66-8966-99F5CF5495A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC84C8-6BD6-4EE8-B2C0-52BFAC4CEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="3204" windowWidth="27264" windowHeight="14892" xr2:uid="{E56D4043-BA5A-4184-995B-D9D6E6830654}"/>
+    <workbookView xWindow="-23136" yWindow="0" windowWidth="23232" windowHeight="25296" xr2:uid="{E56D4043-BA5A-4184-995B-D9D6E6830654}"/>
   </bookViews>
   <sheets>
     <sheet name="dct_analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -306,13 +306,46 @@
   </si>
   <si>
     <t>sampling_year</t>
+  </si>
+  <si>
+    <t>Precision of coordinates</t>
+  </si>
+  <si>
+    <t>substance_id</t>
+  </si>
+  <si>
+    <t>concentration indicator</t>
+  </si>
+  <si>
+    <t>sampling_technique_id</t>
+  </si>
+  <si>
+    <t>method_id</t>
+  </si>
+  <si>
+    <t>data_source_id</t>
+  </si>
+  <si>
+    <t>406 - delete dcod_id = 2</t>
+  </si>
+  <si>
+    <t>availability_id</t>
+  </si>
+  <si>
+    <t>dataset_id</t>
+  </si>
+  <si>
+    <t>merge - sampling technique</t>
+  </si>
+  <si>
+    <t>aky je rozdiel voci data_source_id (riadok 45)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,13 +361,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -346,14 +391,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -686,17 +734,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D3357F-FAFF-4601-99DD-3BC9B1D30FBC}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D71" sqref="A71:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,6 +779,9 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -743,6 +795,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -751,41 +806,65 @@
       <c r="B7" t="s">
         <v>81</v>
       </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -803,7 +882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -811,7 +890,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -819,7 +898,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -827,7 +906,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -835,7 +914,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -843,7 +922,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -851,7 +930,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -859,7 +938,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -867,22 +946,30 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -890,178 +977,247 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="C57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>57</v>
       </c>
       <c r="B60" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -1069,7 +1225,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -1077,7 +1233,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -1085,7 +1241,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -1093,7 +1249,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -1101,7 +1257,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -1109,67 +1265,110 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="B70" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
full structure + stations seeder
</commit_message>
<xml_diff>
--- a/_data/database_tables_upgrades.xlsx
+++ b/_data/database_tables_upgrades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_w\norman-db\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00201d7a97493cc5/web_projects/norman-db/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC84C8-6BD6-4EE8-B2C0-52BFAC4CEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{33AC84C8-6BD6-4EE8-B2C0-52BFAC4CEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D54BAC4-E1ED-46AC-908E-F1D8230418B7}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="0" windowWidth="23232" windowHeight="25296" xr2:uid="{E56D4043-BA5A-4184-995B-D9D6E6830654}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{E56D4043-BA5A-4184-995B-D9D6E6830654}"/>
   </bookViews>
   <sheets>
     <sheet name="dct_analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -305,9 +305,6 @@
     <t>added_by</t>
   </si>
   <si>
-    <t>sampling_year</t>
-  </si>
-  <si>
     <t>Precision of coordinates</t>
   </si>
   <si>
@@ -332,13 +329,43 @@
     <t>availability_id</t>
   </si>
   <si>
-    <t>dataset_id</t>
-  </si>
-  <si>
     <t>merge - sampling technique</t>
   </si>
   <si>
-    <t>aky je rozdiel voci data_source_id (riadok 45)</t>
+    <t>treatment_less_id</t>
+  </si>
+  <si>
+    <t>treatment_less</t>
+  </si>
+  <si>
+    <t>moved to "treatment_less"</t>
+  </si>
+  <si>
+    <t>moved to "remarks" json</t>
+  </si>
+  <si>
+    <t>file_source_id</t>
+  </si>
+  <si>
+    <t>coordinate_precision_id</t>
+  </si>
+  <si>
+    <t>"coordinate_precisions"</t>
+  </si>
+  <si>
+    <t>sampling_date_year</t>
+  </si>
+  <si>
+    <t>sampling_date_month</t>
+  </si>
+  <si>
+    <t>sampling_date_date</t>
+  </si>
+  <si>
+    <t>sampling_date_time</t>
+  </si>
+  <si>
+    <t>concentration_indicator_id</t>
   </si>
 </sst>
 </file>
@@ -415,6 +442,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,14 +767,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D3357F-FAFF-4601-99DD-3BC9B1D30FBC}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D71" sqref="A71:D71"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -780,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -947,13 +978,17 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>90</v>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,7 +1036,7 @@
         <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1009,10 +1044,10 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1038,7 +1073,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1050,21 +1085,33 @@
       <c r="A38" t="s">
         <v>35</v>
       </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -1081,7 +1128,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1089,7 +1136,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1101,11 +1148,17 @@
       <c r="A47" t="s">
         <v>44</v>
       </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -1180,28 +1233,28 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="C59" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="B60" t="s">
-        <v>34</v>
-      </c>
       <c r="C60" t="s">
         <v>83</v>
       </c>
@@ -1210,9 +1263,6 @@
       <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
       <c r="C61" t="s">
         <v>83</v>
       </c>
@@ -1270,7 +1320,7 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1286,22 +1336,18 @@
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="A71" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
-        <v>100</v>
+      <c r="B71" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>